<commit_message>
mudança função excel e correção nome filme
</commit_message>
<xml_diff>
--- a/letterboxd_scraping/reviews.xlsx
+++ b/letterboxd_scraping/reviews.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Filme</t>
+          <t>Movie</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -495,7 +495,11 @@
       <c r="F2" t="n">
         <v>42</v>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H2" t="n">
         <v>-0.58</v>
       </c>
@@ -525,7 +529,11 @@
       <c r="F3" t="n">
         <v>66</v>
       </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H3" t="n">
         <v>0.42</v>
       </c>
@@ -555,7 +563,11 @@
       <c r="F4" t="n">
         <v>22</v>
       </c>
-      <c r="G4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H4" t="n">
         <v>-0.08</v>
       </c>
@@ -585,7 +597,11 @@
       <c r="F5" t="n">
         <v>27</v>
       </c>
-      <c r="G5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H5" t="n">
         <v>-0.08</v>
       </c>
@@ -615,7 +631,11 @@
       <c r="F6" t="n">
         <v>425</v>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H6" t="n">
         <v>0.42</v>
       </c>
@@ -645,7 +665,11 @@
       <c r="F7" t="n">
         <v>45</v>
       </c>
-      <c r="G7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H7" t="n">
         <v>0.42</v>
       </c>
@@ -675,7 +699,11 @@
       <c r="F8" t="n">
         <v>36</v>
       </c>
-      <c r="G8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H8" t="n">
         <v>-0.58</v>
       </c>
@@ -705,7 +733,11 @@
       <c r="F9" t="n">
         <v>139</v>
       </c>
-      <c r="G9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H9" t="n">
         <v>0.42</v>
       </c>
@@ -735,7 +767,11 @@
       <c r="F10" t="n">
         <v>484</v>
       </c>
-      <c r="G10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H10" t="n">
         <v>0.42</v>
       </c>
@@ -765,7 +801,11 @@
       <c r="F11" t="n">
         <v>424</v>
       </c>
-      <c r="G11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H11" t="n">
         <v>-2.58</v>
       </c>
@@ -795,7 +835,11 @@
       <c r="F12" t="n">
         <v>87</v>
       </c>
-      <c r="G12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H12" t="n">
         <v>0.42</v>
       </c>
@@ -825,7 +869,11 @@
       <c r="F13" t="n">
         <v>393</v>
       </c>
-      <c r="G13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H13" t="n">
         <v>0.42</v>
       </c>
@@ -855,7 +903,11 @@
       <c r="F14" t="n">
         <v>79</v>
       </c>
-      <c r="G14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H14" t="n">
         <v>0.42</v>
       </c>
@@ -885,7 +937,11 @@
       <c r="F15" t="n">
         <v>101</v>
       </c>
-      <c r="G15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H15" t="n">
         <v>0.42</v>
       </c>
@@ -915,7 +971,11 @@
       <c r="F16" t="n">
         <v>50</v>
       </c>
-      <c r="G16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H16" t="n">
         <v>0.42</v>
       </c>
@@ -945,7 +1005,11 @@
       <c r="F17" t="n">
         <v>422</v>
       </c>
-      <c r="G17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H17" t="n">
         <v>-0.08</v>
       </c>
@@ -975,7 +1039,11 @@
       <c r="F18" t="n">
         <v>140</v>
       </c>
-      <c r="G18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H18" t="n">
         <v>-0.58</v>
       </c>
@@ -1005,7 +1073,11 @@
       <c r="F19" t="n">
         <v>290</v>
       </c>
-      <c r="G19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H19" t="n">
         <v>0.42</v>
       </c>
@@ -1035,7 +1107,11 @@
       <c r="F20" t="n">
         <v>388</v>
       </c>
-      <c r="G20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H20" t="n">
         <v>-0.08</v>
       </c>
@@ -1065,7 +1141,11 @@
       <c r="F21" t="n">
         <v>100</v>
       </c>
-      <c r="G21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H21" t="n">
         <v>-0.58</v>
       </c>
@@ -1095,7 +1175,11 @@
       <c r="F22" t="n">
         <v>78</v>
       </c>
-      <c r="G22" t="inlineStr"/>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H22" t="n">
         <v>0.42</v>
       </c>
@@ -1125,7 +1209,11 @@
       <c r="F23" t="n">
         <v>549</v>
       </c>
-      <c r="G23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H23" t="n">
         <v>-0.08</v>
       </c>
@@ -1155,7 +1243,11 @@
       <c r="F24" t="n">
         <v>451</v>
       </c>
-      <c r="G24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H24" t="n">
         <v>-0.08</v>
       </c>
@@ -1185,7 +1277,11 @@
       <c r="F25" t="n">
         <v>144</v>
       </c>
-      <c r="G25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/everything-everywhere-all-at-once/</t>
+        </is>
+      </c>
       <c r="H25" t="n">
         <v>0.42</v>
       </c>
@@ -1215,7 +1311,11 @@
       <c r="F26" t="n">
         <v>143</v>
       </c>
-      <c r="G26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H26" t="n">
         <v>0.33</v>
       </c>
@@ -1245,7 +1345,11 @@
       <c r="F27" t="n">
         <v>116</v>
       </c>
-      <c r="G27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H27" t="n">
         <v>0.33</v>
       </c>
@@ -1275,7 +1379,11 @@
       <c r="F28" t="n">
         <v>39</v>
       </c>
-      <c r="G28" t="inlineStr"/>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H28" t="n">
         <v>0.33</v>
       </c>
@@ -1305,7 +1413,11 @@
       <c r="F29" t="n">
         <v>29</v>
       </c>
-      <c r="G29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H29" t="n">
         <v>0.33</v>
       </c>
@@ -1335,7 +1447,11 @@
       <c r="F30" t="n">
         <v>66</v>
       </c>
-      <c r="G30" t="inlineStr"/>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H30" t="n">
         <v>0.33</v>
       </c>
@@ -1365,7 +1481,11 @@
       <c r="F31" t="n">
         <v>506</v>
       </c>
-      <c r="G31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H31" t="n">
         <v>-0.67</v>
       </c>
@@ -1395,7 +1515,11 @@
       <c r="F32" t="n">
         <v>29</v>
       </c>
-      <c r="G32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H32" t="n">
         <v>-0.67</v>
       </c>
@@ -1425,7 +1549,11 @@
       <c r="F33" t="n">
         <v>136</v>
       </c>
-      <c r="G33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H33" t="n">
         <v>0.33</v>
       </c>
@@ -1455,7 +1583,11 @@
       <c r="F34" t="n">
         <v>261</v>
       </c>
-      <c r="G34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H34" t="n">
         <v>-0.17</v>
       </c>
@@ -1485,7 +1617,11 @@
       <c r="F35" t="n">
         <v>549</v>
       </c>
-      <c r="G35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H35" t="n">
         <v>-0.17</v>
       </c>
@@ -1515,7 +1651,11 @@
       <c r="F36" t="n">
         <v>31</v>
       </c>
-      <c r="G36" t="inlineStr"/>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H36" t="n">
         <v>0.33</v>
       </c>
@@ -1545,7 +1685,11 @@
       <c r="F37" t="n">
         <v>291</v>
       </c>
-      <c r="G37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H37" t="n">
         <v>-0.17</v>
       </c>
@@ -1575,7 +1719,11 @@
       <c r="F38" t="n">
         <v>86</v>
       </c>
-      <c r="G38" t="inlineStr"/>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H38" t="n">
         <v>0.33</v>
       </c>
@@ -1605,7 +1753,11 @@
       <c r="F39" t="n">
         <v>166</v>
       </c>
-      <c r="G39" t="inlineStr"/>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H39" t="n">
         <v>-0.67</v>
       </c>
@@ -1635,7 +1787,11 @@
       <c r="F40" t="n">
         <v>33</v>
       </c>
-      <c r="G40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H40" t="n">
         <v>-0.17</v>
       </c>
@@ -1665,7 +1821,11 @@
       <c r="F41" t="n">
         <v>77</v>
       </c>
-      <c r="G41" t="inlineStr"/>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H41" t="n">
         <v>-0.17</v>
       </c>
@@ -1695,7 +1855,11 @@
       <c r="F42" t="n">
         <v>32</v>
       </c>
-      <c r="G42" t="inlineStr"/>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H42" t="n">
         <v>0.33</v>
       </c>
@@ -1725,7 +1889,11 @@
       <c r="F43" t="n">
         <v>51</v>
       </c>
-      <c r="G43" t="inlineStr"/>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H43" t="n">
         <v>-0.17</v>
       </c>
@@ -1755,7 +1923,11 @@
       <c r="F44" t="n">
         <v>180</v>
       </c>
-      <c r="G44" t="inlineStr"/>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H44" t="n">
         <v>0.33</v>
       </c>
@@ -1785,7 +1957,11 @@
       <c r="F45" t="n">
         <v>226</v>
       </c>
-      <c r="G45" t="inlineStr"/>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H45" t="n">
         <v>0.33</v>
       </c>
@@ -1815,7 +1991,11 @@
       <c r="F46" t="n">
         <v>96</v>
       </c>
-      <c r="G46" t="inlineStr"/>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H46" t="n">
         <v>0.33</v>
       </c>
@@ -1845,7 +2025,11 @@
       <c r="F47" t="n">
         <v>153</v>
       </c>
-      <c r="G47" t="inlineStr"/>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H47" t="n">
         <v>-0.67</v>
       </c>
@@ -1875,7 +2059,11 @@
       <c r="F48" t="n">
         <v>50</v>
       </c>
-      <c r="G48" t="inlineStr"/>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-into-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H48" t="n">
         <v>-0.17</v>
       </c>
@@ -1905,7 +2093,11 @@
       <c r="F49" t="n">
         <v>108</v>
       </c>
-      <c r="G49" t="inlineStr"/>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H49" t="n">
         <v>-0.14</v>
       </c>
@@ -1935,7 +2127,11 @@
       <c r="F50" t="n">
         <v>46</v>
       </c>
-      <c r="G50" t="inlineStr"/>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H50" t="n">
         <v>-0.64</v>
       </c>
@@ -1965,7 +2161,11 @@
       <c r="F51" t="n">
         <v>75</v>
       </c>
-      <c r="G51" t="inlineStr"/>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H51" t="n">
         <v>-0.14</v>
       </c>
@@ -1995,7 +2195,11 @@
       <c r="F52" t="n">
         <v>51</v>
       </c>
-      <c r="G52" t="inlineStr"/>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H52" t="n">
         <v>0.36</v>
       </c>
@@ -2025,7 +2229,11 @@
       <c r="F53" t="n">
         <v>35</v>
       </c>
-      <c r="G53" t="inlineStr"/>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H53" t="n">
         <v>0.36</v>
       </c>
@@ -2055,7 +2263,11 @@
       <c r="F54" t="n">
         <v>70</v>
       </c>
-      <c r="G54" t="inlineStr"/>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H54" t="n">
         <v>0.36</v>
       </c>
@@ -2085,7 +2297,11 @@
       <c r="F55" t="n">
         <v>34</v>
       </c>
-      <c r="G55" t="inlineStr"/>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H55" t="n">
         <v>-0.14</v>
       </c>
@@ -2115,7 +2331,11 @@
       <c r="F56" t="n">
         <v>202</v>
       </c>
-      <c r="G56" t="inlineStr"/>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H56" t="n">
         <v>-0.14</v>
       </c>
@@ -2145,7 +2365,11 @@
       <c r="F57" t="n">
         <v>579</v>
       </c>
-      <c r="G57" t="inlineStr"/>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H57" t="n">
         <v>0.36</v>
       </c>
@@ -2175,7 +2399,11 @@
       <c r="F58" t="n">
         <v>29</v>
       </c>
-      <c r="G58" t="inlineStr"/>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H58" t="n">
         <v>-0.64</v>
       </c>
@@ -2205,7 +2433,11 @@
       <c r="F59" t="n">
         <v>238</v>
       </c>
-      <c r="G59" t="inlineStr"/>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H59" t="n">
         <v>0.36</v>
       </c>
@@ -2235,7 +2467,11 @@
       <c r="F60" t="n">
         <v>111</v>
       </c>
-      <c r="G60" t="inlineStr"/>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H60" t="n">
         <v>0.36</v>
       </c>
@@ -2265,7 +2501,11 @@
       <c r="F61" t="n">
         <v>65</v>
       </c>
-      <c r="G61" t="inlineStr"/>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H61" t="n">
         <v>0.36</v>
       </c>
@@ -2295,7 +2535,11 @@
       <c r="F62" t="n">
         <v>94</v>
       </c>
-      <c r="G62" t="inlineStr"/>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H62" t="n">
         <v>0.36</v>
       </c>
@@ -2325,7 +2569,11 @@
       <c r="F63" t="n">
         <v>189</v>
       </c>
-      <c r="G63" t="inlineStr"/>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H63" t="n">
         <v>0.36</v>
       </c>
@@ -2355,7 +2603,11 @@
       <c r="F64" t="n">
         <v>116</v>
       </c>
-      <c r="G64" t="inlineStr"/>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H64" t="n">
         <v>-1.14</v>
       </c>
@@ -2385,7 +2637,11 @@
       <c r="F65" t="n">
         <v>99</v>
       </c>
-      <c r="G65" t="inlineStr"/>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H65" t="n">
         <v>-0.14</v>
       </c>
@@ -2415,7 +2671,11 @@
       <c r="F66" t="n">
         <v>9</v>
       </c>
-      <c r="G66" t="inlineStr"/>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H66" t="n">
         <v>-0.14</v>
       </c>
@@ -2445,7 +2705,11 @@
       <c r="F67" t="n">
         <v>8</v>
       </c>
-      <c r="G67" t="inlineStr"/>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H67" t="n">
         <v>0.36</v>
       </c>
@@ -2475,7 +2739,11 @@
       <c r="F68" t="n">
         <v>60</v>
       </c>
-      <c r="G68" t="inlineStr"/>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H68" t="n">
         <v>-0.64</v>
       </c>
@@ -2505,7 +2773,11 @@
       <c r="F69" t="n">
         <v>72</v>
       </c>
-      <c r="G69" t="inlineStr"/>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/inception/</t>
+        </is>
+      </c>
       <c r="H69" t="n">
         <v>0.36</v>
       </c>
@@ -2535,7 +2807,11 @@
       <c r="F70" t="n">
         <v>355</v>
       </c>
-      <c r="G70" t="inlineStr"/>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H70" t="n">
         <v>0.25</v>
       </c>
@@ -2565,7 +2841,11 @@
       <c r="F71" t="n">
         <v>73</v>
       </c>
-      <c r="G71" t="inlineStr"/>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H71" t="n">
         <v>-0.25</v>
       </c>
@@ -2595,7 +2875,11 @@
       <c r="F72" t="n">
         <v>296</v>
       </c>
-      <c r="G72" t="inlineStr"/>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H72" t="n">
         <v>0.25</v>
       </c>
@@ -2625,7 +2909,11 @@
       <c r="F73" t="n">
         <v>16</v>
       </c>
-      <c r="G73" t="inlineStr"/>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H73" t="n">
         <v>0.25</v>
       </c>
@@ -2655,7 +2943,11 @@
       <c r="F74" t="n">
         <v>170</v>
       </c>
-      <c r="G74" t="inlineStr"/>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H74" t="n">
         <v>0.25</v>
       </c>
@@ -2685,7 +2977,11 @@
       <c r="F75" t="n">
         <v>475</v>
       </c>
-      <c r="G75" t="inlineStr"/>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H75" t="n">
         <v>0.25</v>
       </c>
@@ -2715,7 +3011,11 @@
       <c r="F76" t="n">
         <v>20</v>
       </c>
-      <c r="G76" t="inlineStr"/>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H76" t="n">
         <v>-0.75</v>
       </c>
@@ -2745,7 +3045,11 @@
       <c r="F77" t="n">
         <v>28</v>
       </c>
-      <c r="G77" t="inlineStr"/>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H77" t="n">
         <v>0.25</v>
       </c>
@@ -2775,7 +3079,11 @@
       <c r="F78" t="n">
         <v>96</v>
       </c>
-      <c r="G78" t="inlineStr"/>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H78" t="n">
         <v>-0.75</v>
       </c>
@@ -2805,7 +3113,11 @@
       <c r="F79" t="n">
         <v>26</v>
       </c>
-      <c r="G79" t="inlineStr"/>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H79" t="n">
         <v>0.25</v>
       </c>
@@ -2835,7 +3147,11 @@
       <c r="F80" t="n">
         <v>111</v>
       </c>
-      <c r="G80" t="inlineStr"/>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H80" t="n">
         <v>-0.25</v>
       </c>
@@ -2865,7 +3181,11 @@
       <c r="F81" t="n">
         <v>36</v>
       </c>
-      <c r="G81" t="inlineStr"/>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H81" t="n">
         <v>0.25</v>
       </c>
@@ -2895,7 +3215,11 @@
       <c r="F82" t="n">
         <v>367</v>
       </c>
-      <c r="G82" t="inlineStr"/>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H82" t="n">
         <v>0.25</v>
       </c>
@@ -2925,7 +3249,11 @@
       <c r="F83" t="n">
         <v>45</v>
       </c>
-      <c r="G83" t="inlineStr"/>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H83" t="n">
         <v>0.25</v>
       </c>
@@ -2955,7 +3283,11 @@
       <c r="F84" t="n">
         <v>176</v>
       </c>
-      <c r="G84" t="inlineStr"/>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H84" t="n">
         <v>0.25</v>
       </c>
@@ -2985,7 +3317,11 @@
       <c r="F85" t="n">
         <v>33</v>
       </c>
-      <c r="G85" t="inlineStr"/>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H85" t="n">
         <v>0.25</v>
       </c>
@@ -3015,7 +3351,11 @@
       <c r="F86" t="n">
         <v>92</v>
       </c>
-      <c r="G86" t="inlineStr"/>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H86" t="n">
         <v>0.25</v>
       </c>
@@ -3045,7 +3385,11 @@
       <c r="F87" t="n">
         <v>247</v>
       </c>
-      <c r="G87" t="inlineStr"/>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H87" t="n">
         <v>-1.25</v>
       </c>
@@ -3075,7 +3419,11 @@
       <c r="F88" t="n">
         <v>150</v>
       </c>
-      <c r="G88" t="inlineStr"/>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H88" t="n">
         <v>0.25</v>
       </c>
@@ -3105,7 +3453,11 @@
       <c r="F89" t="n">
         <v>72</v>
       </c>
-      <c r="G89" t="inlineStr"/>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H89" t="n">
         <v>-0.25</v>
       </c>
@@ -3135,7 +3487,11 @@
       <c r="F90" t="n">
         <v>42</v>
       </c>
-      <c r="G90" t="inlineStr"/>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H90" t="n">
         <v>-0.25</v>
       </c>
@@ -3165,7 +3521,11 @@
       <c r="F91" t="n">
         <v>193</v>
       </c>
-      <c r="G91" t="inlineStr"/>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-across-the-spider-verse/</t>
+        </is>
+      </c>
       <c r="H91" t="n">
         <v>0.25</v>
       </c>
@@ -3195,7 +3555,11 @@
       <c r="F92" t="n">
         <v>143</v>
       </c>
-      <c r="G92" t="inlineStr"/>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H92" t="n">
         <v>0.08</v>
       </c>
@@ -3225,7 +3589,11 @@
       <c r="F93" t="n">
         <v>199</v>
       </c>
-      <c r="G93" t="inlineStr"/>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H93" t="n">
         <v>1.58</v>
       </c>
@@ -3255,7 +3623,11 @@
       <c r="F94" t="n">
         <v>508</v>
       </c>
-      <c r="G94" t="inlineStr"/>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H94" t="n">
         <v>-1.42</v>
       </c>
@@ -3285,7 +3657,11 @@
       <c r="F95" t="n">
         <v>197</v>
       </c>
-      <c r="G95" t="inlineStr"/>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H95" t="n">
         <v>1.08</v>
       </c>
@@ -3315,7 +3691,11 @@
       <c r="F96" t="n">
         <v>74</v>
       </c>
-      <c r="G96" t="inlineStr"/>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H96" t="n">
         <v>0.08</v>
       </c>
@@ -3345,7 +3725,11 @@
       <c r="F97" t="n">
         <v>129</v>
       </c>
-      <c r="G97" t="inlineStr"/>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H97" t="n">
         <v>-0.92</v>
       </c>
@@ -3375,7 +3759,11 @@
       <c r="F98" t="n">
         <v>44</v>
       </c>
-      <c r="G98" t="inlineStr"/>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H98" t="n">
         <v>0.08</v>
       </c>
@@ -3405,7 +3793,11 @@
       <c r="F99" t="n">
         <v>45</v>
       </c>
-      <c r="G99" t="inlineStr"/>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H99" t="n">
         <v>1.58</v>
       </c>
@@ -3435,7 +3827,11 @@
       <c r="F100" t="n">
         <v>79</v>
       </c>
-      <c r="G100" t="inlineStr"/>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H100" t="n">
         <v>-1.42</v>
       </c>
@@ -3465,7 +3861,11 @@
       <c r="F101" t="n">
         <v>48</v>
       </c>
-      <c r="G101" t="inlineStr"/>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H101" t="n">
         <v>-1.42</v>
       </c>
@@ -3495,7 +3895,11 @@
       <c r="F102" t="n">
         <v>49</v>
       </c>
-      <c r="G102" t="inlineStr"/>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H102" t="n">
         <v>1.08</v>
       </c>
@@ -3525,7 +3929,11 @@
       <c r="F103" t="n">
         <v>306</v>
       </c>
-      <c r="G103" t="inlineStr"/>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H103" t="n">
         <v>1.58</v>
       </c>
@@ -3555,7 +3963,11 @@
       <c r="F104" t="n">
         <v>435</v>
       </c>
-      <c r="G104" t="inlineStr"/>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H104" t="n">
         <v>-0.92</v>
       </c>
@@ -3585,7 +3997,11 @@
       <c r="F105" t="n">
         <v>135</v>
       </c>
-      <c r="G105" t="inlineStr"/>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H105" t="n">
         <v>-1.42</v>
       </c>
@@ -3615,7 +4031,11 @@
       <c r="F106" t="n">
         <v>531</v>
       </c>
-      <c r="G106" t="inlineStr"/>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H106" t="n">
         <v>0.08</v>
       </c>
@@ -3645,7 +4065,11 @@
       <c r="F107" t="n">
         <v>101</v>
       </c>
-      <c r="G107" t="inlineStr"/>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H107" t="n">
         <v>0.08</v>
       </c>
@@ -3675,7 +4099,11 @@
       <c r="F108" t="n">
         <v>434</v>
       </c>
-      <c r="G108" t="inlineStr"/>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H108" t="n">
         <v>-0.92</v>
       </c>
@@ -3705,7 +4133,11 @@
       <c r="F109" t="n">
         <v>103</v>
       </c>
-      <c r="G109" t="inlineStr"/>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H109" t="n">
         <v>1.08</v>
       </c>
@@ -3735,7 +4167,11 @@
       <c r="F110" t="n">
         <v>140</v>
       </c>
-      <c r="G110" t="inlineStr"/>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H110" t="n">
         <v>0.58</v>
       </c>
@@ -3765,7 +4201,11 @@
       <c r="F111" t="n">
         <v>30</v>
       </c>
-      <c r="G111" t="inlineStr"/>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/spider-man-no-way-home/</t>
+        </is>
+      </c>
       <c r="H111" t="n">
         <v>-0.42</v>
       </c>

</xml_diff>